<commit_message>
adicao do usuario comum
</commit_message>
<xml_diff>
--- a/files/Casos de Uso/Resumo Casos de Uso.xlsx
+++ b/files/Casos de Uso/Resumo Casos de Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
   <si>
     <t>Identificador</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>CSU-33</t>
+  </si>
+  <si>
+    <t>Administrador/Comprador/Organizadora/Usuário Comum</t>
+  </si>
+  <si>
+    <t>Usuário Comum</t>
   </si>
 </sst>
 </file>
@@ -833,14 +839,14 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="23.42578125" style="4"/>
   </cols>
@@ -879,7 +885,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>70</v>
@@ -893,7 +899,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>70</v>
@@ -1113,7 +1119,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>70</v>
@@ -1241,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>70</v>

</xml_diff>